<commit_message>
Reorganize folders; update main fig
</commit_message>
<xml_diff>
--- a/Data/Frahm_HPsub_eco.xlsx
+++ b/Data/Frahm_HPsub_eco.xlsx
@@ -1,18 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Hippo_Eco/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1369D711-8C34-3C4E-900B-BD5D3E63D7E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24540" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24540" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final_Data" sheetId="1" r:id="rId1"/>
     <sheet name="Key" sheetId="2" r:id="rId2"/>
     <sheet name="Stephan_Manoleseu" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Brian Schilder</author>
   </authors>
   <commentList>
-    <comment ref="M3" authorId="0">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -45,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="422">
   <si>
     <t>Subiculum</t>
   </si>
@@ -1032,9 +1044,6 @@
   </si>
   <si>
     <t>Tarsius</t>
-  </si>
-  <si>
-    <t>Species_David</t>
   </si>
   <si>
     <t>Cebus albifrons</t>
@@ -1344,7 +1353,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -2413,6 +2422,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2737,15 +2754,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46:XFD46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
@@ -2755,9 +2772,9 @@
     <col min="84" max="84" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" s="52" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:84" s="52" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>329</v>
+        <v>388</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -2784,7 +2801,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>8</v>
@@ -2793,7 +2810,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="49" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N1" s="50" t="s">
         <v>11</v>
@@ -2802,16 +2819,16 @@
         <v>60</v>
       </c>
       <c r="P1" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q1" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>357</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>358</v>
       </c>
       <c r="T1" s="11" t="s">
         <v>59</v>
@@ -2892,7 +2909,7 @@
         <v>85</v>
       </c>
       <c r="AT1" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AU1" s="12" t="s">
         <v>86</v>
@@ -2994,7 +3011,7 @@
         <v>118</v>
       </c>
       <c r="CB1" s="42" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="CC1" s="42" t="s">
         <v>119</v>
@@ -3006,10 +3023,10 @@
         <v>121</v>
       </c>
       <c r="CF1" s="51" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
-    <row r="2" spans="1:84">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
@@ -3056,7 +3073,7 @@
         <v>123</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q2" s="4">
         <v>52</v>
@@ -3077,13 +3094,13 @@
         <v>125</v>
       </c>
       <c r="W2" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="X2" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>344</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>345</v>
       </c>
       <c r="Z2" s="4">
         <v>3</v>
@@ -3176,7 +3193,7 @@
         <v>124</v>
       </c>
       <c r="BD2" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="BE2" s="4" t="s">
         <v>124</v>
@@ -3269,7 +3286,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:84">
+    <row r="3" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -3527,7 +3544,7 @@
         <v>157.5</v>
       </c>
     </row>
-    <row r="4" spans="1:84">
+    <row r="4" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -3790,7 +3807,7 @@
         <v>11.759626130244845</v>
       </c>
     </row>
-    <row r="5" spans="1:84">
+    <row r="5" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -4049,7 +4066,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:84">
+    <row r="6" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -4096,7 +4113,7 @@
         <v>18</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q6" s="4">
         <v>9.67</v>
@@ -4309,7 +4326,7 @@
         <v>291.97080291970804</v>
       </c>
     </row>
-    <row r="7" spans="1:84">
+    <row r="7" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -4567,7 +4584,7 @@
         <v>147.5</v>
       </c>
     </row>
-    <row r="8" spans="1:84">
+    <row r="8" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -4828,7 +4845,7 @@
         <v>5.8606811145510829</v>
       </c>
     </row>
-    <row r="9" spans="1:84">
+    <row r="9" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -5089,7 +5106,7 @@
         <v>217.37288135593221</v>
       </c>
     </row>
-    <row r="10" spans="1:84">
+    <row r="10" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
@@ -5136,7 +5153,7 @@
         <v>22</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q10" s="4">
         <v>4.5</v>
@@ -5349,7 +5366,7 @@
         <v>1538.2352941176471</v>
       </c>
     </row>
-    <row r="11" spans="1:84" s="1" customFormat="1">
+    <row r="11" spans="1:84" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>23</v>
       </c>
@@ -5417,13 +5434,13 @@
         <v>125</v>
       </c>
       <c r="W11" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="X11" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="X11" s="4" t="s">
-        <v>342</v>
-      </c>
       <c r="Y11" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Z11" s="4">
         <v>3</v>
@@ -5516,7 +5533,7 @@
         <v>124</v>
       </c>
       <c r="BD11" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="BE11" s="4" t="s">
         <v>124</v>
@@ -5609,7 +5626,7 @@
         <v>15.925925925925926</v>
       </c>
     </row>
-    <row r="12" spans="1:84">
+    <row r="12" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
@@ -5872,7 +5889,7 @@
         <v>63.7516688918558</v>
       </c>
     </row>
-    <row r="13" spans="1:84">
+    <row r="13" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>25</v>
       </c>
@@ -6135,7 +6152,7 @@
         <v>27.952999381570809</v>
       </c>
     </row>
-    <row r="14" spans="1:84">
+    <row r="14" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>26</v>
       </c>
@@ -6393,7 +6410,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:84">
+    <row r="15" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
@@ -6652,7 +6669,7 @@
         <v>158.73015873015873</v>
       </c>
     </row>
-    <row r="16" spans="1:84">
+    <row r="16" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
@@ -6912,7 +6929,7 @@
         <v>0.97418412079883099</v>
       </c>
     </row>
-    <row r="17" spans="1:84">
+    <row r="17" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
@@ -7173,7 +7190,7 @@
         <v>0.92537313432835822</v>
       </c>
     </row>
-    <row r="18" spans="1:84">
+    <row r="18" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
@@ -7436,7 +7453,7 @@
         <v>121.94690265486727</v>
       </c>
     </row>
-    <row r="19" spans="1:84">
+    <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
@@ -7695,7 +7712,7 @@
         <v>34.375</v>
       </c>
     </row>
-    <row r="20" spans="1:84">
+    <row r="20" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
@@ -7954,7 +7971,7 @@
         <v>307.69230769230768</v>
       </c>
     </row>
-    <row r="21" spans="1:84">
+    <row r="21" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
@@ -8217,7 +8234,7 @@
         <v>74.95741056218057</v>
       </c>
     </row>
-    <row r="22" spans="1:84">
+    <row r="22" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -8476,7 +8493,7 @@
         <v>14.857142857142858</v>
       </c>
     </row>
-    <row r="23" spans="1:84">
+    <row r="23" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
@@ -8739,7 +8756,7 @@
         <v>13.009900990099009</v>
       </c>
     </row>
-    <row r="24" spans="1:84">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
@@ -8997,7 +9014,7 @@
         <v>11.111111111111111</v>
       </c>
     </row>
-    <row r="25" spans="1:84">
+    <row r="25" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>38</v>
       </c>
@@ -9260,7 +9277,7 @@
         <v>6.4705882352941178</v>
       </c>
     </row>
-    <row r="26" spans="1:84">
+    <row r="26" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
@@ -9517,7 +9534,7 @@
         <v>122.95081967213116</v>
       </c>
     </row>
-    <row r="27" spans="1:84">
+    <row r="27" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>40</v>
       </c>
@@ -9780,7 +9797,7 @@
         <v>6.8281972869128849</v>
       </c>
     </row>
-    <row r="28" spans="1:84">
+    <row r="28" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>41</v>
       </c>
@@ -10039,7 +10056,7 @@
         <v>92.307692307692307</v>
       </c>
     </row>
-    <row r="29" spans="1:84">
+    <row r="29" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>42</v>
       </c>
@@ -10298,7 +10315,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="30" spans="1:84">
+    <row r="30" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
@@ -10556,7 +10573,7 @@
         <v>112.5925925925926</v>
       </c>
     </row>
-    <row r="31" spans="1:84">
+    <row r="31" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
@@ -10817,7 +10834,7 @@
         <v>3.4849065440456419</v>
       </c>
     </row>
-    <row r="32" spans="1:84">
+    <row r="32" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>45</v>
       </c>
@@ -11076,7 +11093,7 @@
         <v>10.989010989010989</v>
       </c>
     </row>
-    <row r="33" spans="1:84">
+    <row r="33" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
@@ -11334,7 +11351,7 @@
         <v>58.333333333333336</v>
       </c>
     </row>
-    <row r="34" spans="1:84">
+    <row r="34" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
@@ -11597,7 +11614,7 @@
         <v>303.08092485549128</v>
       </c>
     </row>
-    <row r="35" spans="1:84">
+    <row r="35" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>48</v>
       </c>
@@ -11860,7 +11877,7 @@
         <v>2.2406275468622656</v>
       </c>
     </row>
-    <row r="36" spans="1:84">
+    <row r="36" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>49</v>
       </c>
@@ -12118,7 +12135,7 @@
         <v>7.1428571428571423</v>
       </c>
     </row>
-    <row r="37" spans="1:84">
+    <row r="37" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
@@ -12381,7 +12398,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="38" spans="1:84">
+    <row r="38" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>51</v>
       </c>
@@ -12640,7 +12657,7 @@
         <v>40.206185567010316</v>
       </c>
     </row>
-    <row r="39" spans="1:84">
+    <row r="39" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>52</v>
       </c>
@@ -12902,7 +12919,7 @@
         <v>106.4269267235541</v>
       </c>
     </row>
-    <row r="40" spans="1:84">
+    <row r="40" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>53</v>
       </c>
@@ -13161,7 +13178,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="41" spans="1:84">
+    <row r="41" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>54</v>
       </c>
@@ -13232,10 +13249,10 @@
         <v>316</v>
       </c>
       <c r="X41" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="Y41" s="4" t="s">
         <v>335</v>
-      </c>
-      <c r="Y41" s="4" t="s">
-        <v>336</v>
       </c>
       <c r="Z41" s="4">
         <v>3</v>
@@ -13328,7 +13345,7 @@
         <v>124</v>
       </c>
       <c r="BD41" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="BE41" s="4" t="s">
         <v>124</v>
@@ -13421,7 +13438,7 @@
         <v>20.757020757020758</v>
       </c>
     </row>
-    <row r="42" spans="1:84">
+    <row r="42" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
@@ -13679,7 +13696,7 @@
         <v>25.641025641025642</v>
       </c>
     </row>
-    <row r="43" spans="1:84">
+    <row r="43" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>56</v>
       </c>
@@ -13940,7 +13957,7 @@
         <v>13.605442176870749</v>
       </c>
     </row>
-    <row r="44" spans="1:84">
+    <row r="44" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>57</v>
       </c>
@@ -14011,10 +14028,10 @@
         <v>328</v>
       </c>
       <c r="X44" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="Y44" s="4" t="s">
         <v>338</v>
-      </c>
-      <c r="Y44" s="4" t="s">
-        <v>339</v>
       </c>
       <c r="Z44" s="4">
         <v>1</v>
@@ -14107,7 +14124,7 @@
         <v>124</v>
       </c>
       <c r="BD44" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BE44" s="4" t="s">
         <v>124</v>
@@ -14201,7 +14218,7 @@
         <v>60.439560439560445</v>
       </c>
     </row>
-    <row r="45" spans="1:84">
+    <row r="45" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>58</v>
       </c>
@@ -14476,14 +14493,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView topLeftCell="C5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.5" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" style="21" customWidth="1"/>
@@ -14494,228 +14511,228 @@
     <col min="7" max="16384" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="16" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F1" s="18"/>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="F2" s="39" t="s">
         <v>364</v>
       </c>
-      <c r="F2" s="39" t="s">
-        <v>365</v>
-      </c>
       <c r="G2" s="40" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="36" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="36" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="36" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45">
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="46" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="36" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="C7" s="55" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="36" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="35" t="s">
+        <v>367</v>
+      </c>
+      <c r="G7" s="41" t="s">
         <v>368</v>
       </c>
-      <c r="G7" s="41" t="s">
-        <v>369</v>
-      </c>
     </row>
-    <row r="8" spans="1:7" ht="30">
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="C8" s="56" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D8" s="30"/>
       <c r="E8" s="37" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G8" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="C9" s="57" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="37" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="35" t="s">
+        <v>373</v>
+      </c>
+      <c r="G9" s="41" t="s">
         <v>374</v>
       </c>
-      <c r="G9" s="41" t="s">
-        <v>375</v>
-      </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="C10" s="18"/>
       <c r="D10" s="23"/>
       <c r="E10" s="37" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="270">
+    <row r="11" spans="1:7" ht="306" x14ac:dyDescent="0.2">
       <c r="C11" s="18"/>
       <c r="D11" s="23"/>
       <c r="E11" s="37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="C12" s="18"/>
       <c r="D12" s="23"/>
       <c r="E12" s="37" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="C13" s="18"/>
       <c r="D13" s="23"/>
       <c r="E13" s="37" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="90">
+    <row r="14" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="C14" s="18"/>
       <c r="D14" s="23"/>
       <c r="E14" s="38" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="31"/>
       <c r="B15" s="32"/>
       <c r="C15" s="33"/>
       <c r="D15" s="34"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C16" s="18"/>
       <c r="D16" s="23"/>
     </row>
@@ -14731,7 +14748,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14739,16 +14756,16 @@
       <selection pane="topRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
     <col min="28" max="29" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="72" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C1" s="72"/>
       <c r="D1" s="72"/>
@@ -14765,7 +14782,7 @@
       <c r="O1" s="72"/>
       <c r="P1" s="72"/>
       <c r="Q1" s="73" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="R1" s="73"/>
       <c r="S1" s="73"/>
@@ -14778,13 +14795,13 @@
       <c r="Z1" s="73"/>
       <c r="AA1" s="73"/>
       <c r="AB1" s="74" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AC1" s="74"/>
     </row>
-    <row r="2" spans="1:30" s="64" customFormat="1">
+    <row r="2" spans="1:30" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="65" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C2" s="65"/>
       <c r="D2" s="65"/>
@@ -14792,22 +14809,22 @@
       <c r="F2" s="65"/>
       <c r="G2" s="65"/>
       <c r="H2" s="66" t="s">
+        <v>398</v>
+      </c>
+      <c r="I2" s="67" t="s">
         <v>399</v>
-      </c>
-      <c r="I2" s="67" t="s">
-        <v>400</v>
       </c>
       <c r="J2" s="67"/>
       <c r="K2" s="67"/>
       <c r="L2" s="68" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M2" s="68"/>
       <c r="N2" s="68"/>
       <c r="O2" s="68"/>
       <c r="P2" s="68"/>
       <c r="Q2" s="77" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R2" s="77"/>
       <c r="S2" s="77"/>
@@ -14822,54 +14839,54 @@
       <c r="AB2" s="70"/>
       <c r="AC2" s="70"/>
     </row>
-    <row r="3" spans="1:30" s="59" customFormat="1" ht="76" thickBot="1">
+    <row r="3" spans="1:30" s="59" customFormat="1" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>396</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>401</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>400</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>402</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>403</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>404</v>
+      </c>
+      <c r="H3" s="61" t="s">
         <v>389</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>397</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>402</v>
-      </c>
-      <c r="D3" s="60" t="s">
-        <v>401</v>
-      </c>
-      <c r="E3" s="60" t="s">
-        <v>403</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>404</v>
-      </c>
-      <c r="G3" s="60" t="s">
+      <c r="I3" s="62" t="s">
+        <v>392</v>
+      </c>
+      <c r="J3" s="62" t="s">
+        <v>390</v>
+      </c>
+      <c r="K3" s="62" t="s">
+        <v>391</v>
+      </c>
+      <c r="L3" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="M3" s="63" t="s">
         <v>405</v>
-      </c>
-      <c r="H3" s="61" t="s">
-        <v>390</v>
-      </c>
-      <c r="I3" s="62" t="s">
-        <v>393</v>
-      </c>
-      <c r="J3" s="62" t="s">
-        <v>391</v>
-      </c>
-      <c r="K3" s="62" t="s">
-        <v>392</v>
-      </c>
-      <c r="L3" s="63" t="s">
-        <v>394</v>
-      </c>
-      <c r="M3" s="63" t="s">
-        <v>406</v>
       </c>
       <c r="N3" s="63" t="s">
         <v>1</v>
       </c>
       <c r="O3" s="63" t="s">
+        <v>394</v>
+      </c>
+      <c r="P3" s="63" t="s">
         <v>395</v>
-      </c>
-      <c r="P3" s="63" t="s">
-        <v>396</v>
       </c>
       <c r="Q3" s="15" t="s">
         <v>0</v>
@@ -14896,7 +14913,7 @@
         <v>7</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="Z3" s="10" t="s">
         <v>8</v>
@@ -14905,18 +14922,18 @@
         <v>9</v>
       </c>
       <c r="AB3" s="49" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AC3" s="75" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AD3" s="59" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B4">
         <v>170</v>
@@ -15002,9 +15019,9 @@
         <v>31.03</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B5">
         <v>852</v>
@@ -15090,9 +15107,9 @@
         <v>40.183000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B6">
         <v>852</v>
@@ -15183,46 +15200,46 @@
         <v>46.190000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="E11">
         <f>100-(Z6/G6*100)</f>
         <v>12.91608391608392</v>
       </c>
       <c r="G11" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
         <v>413</v>
       </c>
+      <c r="G14" t="s">
+        <v>415</v>
+      </c>
     </row>
-    <row r="12" spans="1:30">
-      <c r="H12" t="s">
-        <v>415</v>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>418</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
-      <c r="G13" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30">
-      <c r="F14" t="s">
-        <v>414</v>
-      </c>
-      <c r="G14" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30">
-      <c r="G16" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>